<commit_message>
Cookies to Sessions & Delete Features
</commit_message>
<xml_diff>
--- a/website/static/downloadable_files/Income Expense Query.xlsx
+++ b/website/static/downloadable_files/Income Expense Query.xlsx
@@ -7,88 +7,73 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Income Expense Query" sheetId="1" r:id="rId1"/>
+    <sheet name="Income Expense" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Project Code</t>
-  </si>
-  <si>
-    <t>Project Name</t>
-  </si>
-  <si>
-    <t>Cash Type</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Machine Name</t>
-  </si>
-  <si>
-    <t>Invoice No</t>
-  </si>
-  <si>
-    <t>Qty</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>Remark</t>
-  </si>
-  <si>
-    <t>DCO/23/10/000042</t>
-  </si>
-  <si>
-    <t>PTG-23-24-001</t>
-  </si>
-  <si>
-    <t>Shan - Yet Souk - Kyine Kham Ta Man (23-24)</t>
-  </si>
-  <si>
-    <t>Expense</t>
-  </si>
-  <si>
-    <t>စက်ပြင်စရိတ်</t>
-  </si>
-  <si>
-    <t>KOBELCO-220-02-10445</t>
-  </si>
-  <si>
-    <t>tt-2</t>
-  </si>
-  <si>
-    <t>ထမင်းစရိတ်</t>
-  </si>
-  <si>
-    <t>tt-1</t>
-  </si>
-  <si>
-    <t>DCI/23/10/000041</t>
-  </si>
-  <si>
-    <t>Income</t>
-  </si>
-  <si>
-    <t>ရုံးချုပ်မှ ရငွေ</t>
-  </si>
-  <si>
-    <t>tt-223`</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t xml:space="preserve"> WWW-23-24-003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ချောင်းညီအကိုတာ တာပုံစံကျ ပြန်လည်ပြုပြင်ခြင်း (RD-0+000 to RD-47+520) </t>
+  </si>
+  <si>
+    <t>နေ့စဉ်ငွေ အဝင်အထွက်စာရင်း</t>
+  </si>
+  <si>
+    <t>နေ့စွဲ</t>
+  </si>
+  <si>
+    <t>အကြောင်းအရာ</t>
+  </si>
+  <si>
+    <t>ဘောင်ချာ</t>
+  </si>
+  <si>
+    <t>အဝင်</t>
+  </si>
+  <si>
+    <t>အထွက်</t>
+  </si>
+  <si>
+    <t>လက်ကျန်</t>
+  </si>
+  <si>
+    <t>မှတ်ချက်</t>
+  </si>
+  <si>
+    <t>Opening လက်ကျန်ငွေ</t>
+  </si>
+  <si>
+    <t>ရုံးမှထုတ်ယူငွေ</t>
+  </si>
+  <si>
+    <t>ရုံးမှငွေသားထုတ်ယူခြင်း</t>
+  </si>
+  <si>
+    <t>စားစရိတ်(၂)ဦး နေ့လည်စာ</t>
+  </si>
+  <si>
+    <t>စားစရိတ်(၄)ဦး ညစာ</t>
+  </si>
+  <si>
+    <t>လှိုင်သာယာ တိုးဂိတ် 5B/9222</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>စားစရတ်(၄)ဦး</t>
+  </si>
+  <si>
+    <t>ရေသန့်(၂)ဗူးလဲ</t>
+  </si>
+  <si>
+    <t>စုစုပေါင်း</t>
   </si>
 </sst>
 </file>
@@ -431,150 +416,197 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>45272</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2">
-        <v>45213</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C5" s="1"/>
+      <c r="D5">
+        <v>300000</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>300000</v>
+      </c>
+      <c r="G5" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>45272</v>
+      </c>
+      <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>6000</v>
+      </c>
+      <c r="F6">
+        <v>294000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>45272</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>12000</v>
+      </c>
+      <c r="F7">
+        <v>282000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>45272</v>
+      </c>
+      <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>300</v>
+      </c>
+      <c r="F8">
+        <v>281700</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>45273</v>
+      </c>
+      <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="H2" t="s">
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>28000</v>
+      </c>
+      <c r="F9">
+        <v>253700</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>45273</v>
+      </c>
+      <c r="B10" t="s">
         <v>18</v>
       </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>50000</v>
-      </c>
-      <c r="K2">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3">
-        <v>45213</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>2000</v>
+      </c>
+      <c r="F10">
+        <v>251700</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3">
-        <v>123</v>
-      </c>
-      <c r="J3">
-        <v>50</v>
-      </c>
-      <c r="K3">
-        <v>6150</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4">
-        <v>45213</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>100000</v>
-      </c>
-      <c r="K4">
-        <v>100000</v>
+      <c r="D11">
+        <v>300000</v>
+      </c>
+      <c r="E11">
+        <v>48300</v>
+      </c>
+      <c r="F11">
+        <v>251700</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>